<commit_message>
Modified general crawler, add initial tests
</commit_message>
<xml_diff>
--- a/inflation-resources/data/links.xlsx
+++ b/inflation-resources/data/links.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
-    <t xml:space="preserve">Í</t>
-  </si>
-  <si>
-    <t xml:space="preserve">turkstat_item_name</t>
+    <t xml:space="preserve">item_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item_name</t>
   </si>
   <si>
     <t xml:space="preserve">product_names</t>
@@ -179,6 +179,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -202,12 +203,6 @@
       <charset val="162"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -229,9 +224,16 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -280,12 +282,12 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -293,15 +295,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -309,14 +315,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -329,11 +327,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -361,13 +359,13 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.91"/>
   </cols>
@@ -393,10 +391,10 @@
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -407,10 +405,10 @@
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -421,10 +419,10 @@
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -435,10 +433,10 @@
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -449,10 +447,10 @@
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -463,10 +461,10 @@
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -477,10 +475,10 @@
       <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -491,10 +489,10 @@
       <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -505,10 +503,10 @@
       <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -519,10 +517,10 @@
       <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -533,10 +531,10 @@
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -547,10 +545,10 @@
       <c r="B13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -561,10 +559,10 @@
       <c r="B14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -575,10 +573,10 @@
       <c r="B15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>41</v>
       </c>
     </row>
@@ -589,10 +587,10 @@
       <c r="B16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -603,10 +601,10 @@
       <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>45</v>
       </c>
     </row>
@@ -617,10 +615,10 @@
       <c r="B18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>